<commit_message>
Add Orange Book reference fields to FieldDownload component
</commit_message>
<xml_diff>
--- a/static/fields/drugorangebook_reference.xlsx
+++ b/static/fields/drugorangebook_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11130"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackfinch/WebstormProjects/open.fda.gov/static/fields/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/violet.wren/WebstormProjects/open.fda.gov/static/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEA25AD8-4947-254C-9F08-85C68F447CC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EDB2BD-935B-8A45-B561-79BE0D58B2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drug_label_fields" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Field Name</t>
   </si>
@@ -45,104 +45,19 @@
     <t>Section</t>
   </si>
   <si>
-    <t>OpenFDA fields</t>
-  </si>
-  <si>
     <t>application_number</t>
   </si>
   <si>
     <t>brand_name</t>
   </si>
   <si>
-    <t>generic_name</t>
-  </si>
-  <si>
-    <t>manufacturer_name</t>
-  </si>
-  <si>
-    <t>nui</t>
-  </si>
-  <si>
-    <t>package_ndc</t>
-  </si>
-  <si>
-    <t>array of strings</t>
-  </si>
-  <si>
-    <t>product_ndc</t>
-  </si>
-  <si>
     <t>route</t>
   </si>
   <si>
-    <t>rxcui</t>
-  </si>
-  <si>
-    <t>spl_id</t>
-  </si>
-  <si>
-    <t>spl_set_id</t>
-  </si>
-  <si>
-    <t>substance_name</t>
-  </si>
-  <si>
-    <t>unii</t>
-  </si>
-  <si>
-    <t>This corresponds to the NDA, ANDA, or BLA number reported by the labeler for products which have the corresponding Marketing Category designated. If the designated Marketing Category is OTC Monograph Final or OTC Monograph Not Final, then the application number will be the CFR citation corresponding to the appropriate Monograph (e.g. “part 341”). For unapproved drugs, this field will be null.
-Values follow this pattern:
-^[BLA|ANDA|NDA]{3,4}[0-9]{6}$</t>
-  </si>
-  <si>
     <t>Brand or trade name of the drug product.</t>
   </si>
   <si>
-    <t>Generic name(s) of the drug product.</t>
-  </si>
-  <si>
-    <t>Name of manufacturer or company that makes this drug product, corresponding to the labeler code segment of the NDC.</t>
-  </si>
-  <si>
-    <t>Unique identifier applied to a drug concept within the National Drug File Reference Terminology (NDF-RT).
-Values follow this pattern:
-^[N][0-9]{10}$</t>
-  </si>
-  <si>
-    <t>This number, known as the NDC, identifies the labeler, product, and trade package size. The first segment, the labeler code, is assigned by the FDA. A labeler is any firm that manufactures (including repackers or relabelers), or distributes (under its own name) the drug.
-Values follow this pattern:
-^[0-9]{5,4}-[0-9]{4,3}-[0-9]{1,2}$</t>
-  </si>
-  <si>
-    <t>The labeler manufacturer code and product code segments of the NDC number, separated by a hyphen.
-Values follow this pattern:
-^[0-9]{5,4}-[0-9]{4,3}$</t>
-  </si>
-  <si>
     <t>The route of administation of the drug product.</t>
-  </si>
-  <si>
-    <t>The RxNorm Concept Unique Identifier. RxCUI is a unique number that describes a semantic concept about the drug product, including its ingredients, strength, and dose forms.
-Values follow this pattern:
-^[0-9]{6}$</t>
-  </si>
-  <si>
-    <t>Unique identifier for a particular version of a Structured Product Label for a product. Also referred to as the document ID.
-Values follow this pattern:
-^[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[a-fA-F0-9]{4}-[a-fA-F0-9]{4}-[a-fA-F0-9]{12}$</t>
-  </si>
-  <si>
-    <t>Unique identifier for the Structured Product Label for a product, which is stable across versions of the label. Also referred to as the set ID.
-Values follow this pattern:
-^[a-fA-F0-9]{8}-[a-fA-F0-9]{4}-[a-fA-F0-9]{4}-[a-fA-F0-9]{4}-[a-fA-F0-9]{12}$</t>
-  </si>
-  <si>
-    <t>The list of active ingredients of a drug product.</t>
-  </si>
-  <si>
-    <t>Unique Ingredient Identifier, which is a non-proprietary, free, unique, unambiguous, non-semantic, alphanumeric identifier based on a substance’s molecular structure and/or descriptive information.
-Values follow this pattern:
-^[A-Z0-9]{10}$</t>
   </si>
   <si>
     <t>Active Ingredients</t>
@@ -443,25 +358,25 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -901,18 +816,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="107.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="76.33203125" style="5" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -932,162 +847,162 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,332 +1013,140 @@
         <v>3</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="52" fitToHeight="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="52" fitToHeight="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>